<commit_message>
Update Bug reports table samples.xlsx
Finished uploading all the bug report samples.
</commit_message>
<xml_diff>
--- a/Bug reports table samples.xlsx
+++ b/Bug reports table samples.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="28695" windowHeight="12795"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="28695" windowHeight="12795" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="140">
   <si>
     <t>Description</t>
   </si>
@@ -275,6 +274,232 @@
   </si>
   <si>
     <t>The user is not able to see any of the pages mentioned as shown in the screenshot attached.</t>
+  </si>
+  <si>
+    <t>Chat message typo within tutorial</t>
+  </si>
+  <si>
+    <t>Upon entering any command in the chat you get an error message that has a small typo as seen in the attached image.</t>
+  </si>
+  <si>
+    <t>1. Create a new account on server.
+2. Spawn on the map.
+3. Try to input any command in the chat.</t>
+  </si>
+  <si>
+    <t>The error message should be displayed without the typo.</t>
+  </si>
+  <si>
+    <t>The error message displays with a typo at "com*ands"</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/DzUqwXH.jpeg</t>
+  </si>
+  <si>
+    <t>Email account link to ucp bug</t>
+  </si>
+  <si>
+    <t>Upon trying to link an e-mail account to the ucp account the ucp crashes.</t>
+  </si>
+  <si>
+    <t>1. Visit ucp-beta.liberty.mp
+2. Log in with a valid account.
+3. Go to profile section
+4. Right click on the profile settings wheel.
+5. Go through the e-mail linking.</t>
+  </si>
+  <si>
+    <t>The user should be able to link an e-mail account without crashing the live product.</t>
+  </si>
+  <si>
+    <t>The user is able to crash the live product upon trying to link an email account.</t>
+  </si>
+  <si>
+    <t>GUI bug on 1366x768</t>
+  </si>
+  <si>
+    <t>P3 - low</t>
+  </si>
+  <si>
+    <t>P1 - CRITICAL</t>
+  </si>
+  <si>
+    <t>P2 - HIGH</t>
+  </si>
+  <si>
+    <t>P3 - Medium</t>
+  </si>
+  <si>
+    <t>P4 - Low</t>
+  </si>
+  <si>
+    <t>The GUI is missing the chat message color upon changing the resolution to 1366x768 as shown in the attached screenshot.</t>
+  </si>
+  <si>
+    <t>1. Log onto the server.
+2. Change the game resolution to 1366x768
+3. Click on the chat settings button.</t>
+  </si>
+  <si>
+    <t>The user should have all the chat settings visibible on any resolution.</t>
+  </si>
+  <si>
+    <t>The user is not able to see the last section titled "chat messages color".</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/reQcHG2.jpg
+https://i.imgur.com/vPGgVqx.jpg</t>
+  </si>
+  <si>
+    <t>ATM bug on stealing</t>
+  </si>
+  <si>
+    <t>ATM bug on appearance</t>
+  </si>
+  <si>
+    <t>User is able to steal a an atm that has been already stole and hasn't passed the right amount of time.</t>
+  </si>
+  <si>
+    <t>1. Log onto the server.
+2. Get a personal car.
+3. Get 2 hooks and 1 rope.
+3. Find an ATM on the map that has been stolen already and drive to it.
+4. Park the car near the atm and try to rob it.</t>
+  </si>
+  <si>
+    <t>The user should not be able to steal already stolen ATMs.</t>
+  </si>
+  <si>
+    <t>The user is able to steal already stolen ATMs.</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/XJxwB6V.jpg</t>
+  </si>
+  <si>
+    <t>Upon trying to rob an atm the hook placed between the atm and the car is not placed corectly.</t>
+  </si>
+  <si>
+    <t>1. Log onto the server.
+2. Get a personal car.
+3. Get 2 hooks and 1 rope.
+3. Find an ATM.
+4. Park the car near the atm and try to rob it.</t>
+  </si>
+  <si>
+    <t>The hook should be attatched corectly to the car and the atm.</t>
+  </si>
+  <si>
+    <t>The hook is not attached corectly as shown in the attatched screenshot.</t>
+  </si>
+  <si>
+    <t>Incorect preview on clothing store items.</t>
+  </si>
+  <si>
+    <t>Some items from the clothing store have the wrong image as preview as shown in the attached screenshot.</t>
+  </si>
+  <si>
+    <t>1. Log onto the server.
+2. Go to a clothing store.
+3. Open the menu.</t>
+  </si>
+  <si>
+    <t>The user should see all the clothing items with the correct preview image in the menu and on the character.</t>
+  </si>
+  <si>
+    <t>The user can't see the right clothing image on the menu instead he sees a general placeholder.</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/PjEwMef.jpg</t>
+  </si>
+  <si>
+    <t>Faction garage bug</t>
+  </si>
+  <si>
+    <t>Upon trying to get inside a faction garage with a faction vehicle and someone as a passanger the other person is left on the map with his virtual world changed.</t>
+  </si>
+  <si>
+    <t>1. Log onto the server.
+2. Get a faction car and a passager.
+3. Drive to the faction garage and try to enter with the passager.</t>
+  </si>
+  <si>
+    <t>faction: hitman</t>
+  </si>
+  <si>
+    <t>The user shouldl either get an error saying he can't get inside the garage with the passager OR both players should be teleported inside corectly.</t>
+  </si>
+  <si>
+    <t>The driver gets tp'ed corectly while the passanger isn't.</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/JRfzca6.jpg</t>
+  </si>
+  <si>
+    <t>faction: Varrios Los Astecas</t>
+  </si>
+  <si>
+    <t>Message typo trying to plant weed</t>
+  </si>
+  <si>
+    <t>Upon trying to plant weed outside the designated area the user gets an error message with a typo.</t>
+  </si>
+  <si>
+    <t>1. Log onto the server.
+2. Get inside a gang faction.
+3. Get some weed seeds.
+4. Try to plant anywhere outside the designated areas.</t>
+  </si>
+  <si>
+    <t>The user should be prompted with an error message without the typo.</t>
+  </si>
+  <si>
+    <t>The user is prompted with a message with a typo.</t>
+  </si>
+  <si>
+    <t>Forum last message sent discrepancy</t>
+  </si>
+  <si>
+    <t>As shown in the screenshots attached the author of the last message posted on the forum topic is not displayed corectly.</t>
+  </si>
+  <si>
+    <t>1. Visit ucp-beta.liberty.mp
+2. Log in with a valid account.
+3. Go to the forums section.
+4. Go to "Discutii joc" and create a topic.
+5. Ask 3 people to post a message.
+6. Observe how the author of last message is displayed.</t>
+  </si>
+  <si>
+    <t>The last reply on the topic should be displayed corectly.</t>
+  </si>
+  <si>
+    <t>The last reply on the topic is not displayed corectly.</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/89wCmiK.png
+https://i.imgur.com/3XqKZrq.png
+https://i.imgur.com/bJE4wce.png</t>
+  </si>
+  <si>
+    <t>Profile dropdown menu overlapping server world map</t>
+  </si>
+  <si>
+    <t>As shown in the attached screenshot the dropdown menu of the profile overlaps with the server world map.</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/uIvp8gy.png</t>
+  </si>
+  <si>
+    <t>1. Visit ucp.liberty.mp
+2. Log in with a valid account.
+3. Click on "more" -&gt; "server map".
+4. Click on the dropdown menu.</t>
+  </si>
+  <si>
+    <t>The dropdown menu should be displayed over the map.</t>
+  </si>
+  <si>
+    <t>The dropdown menu is overlapping incorectly.</t>
   </si>
 </sst>
 </file>
@@ -359,7 +584,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -385,6 +610,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -681,10 +912,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView topLeftCell="A22" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -750,7 +981,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="102">
+    <row r="3" spans="1:9" ht="114.75">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -875,7 +1106,7 @@
       <c r="H7" s="7"/>
       <c r="I7" s="8"/>
     </row>
-    <row r="8" spans="1:9" ht="89.25">
+    <row r="8" spans="1:9" ht="102">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -1031,50 +1262,389 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" ht="76.5">
       <c r="A14" s="4">
         <v>13</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
+      <c r="B14" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>80</v>
+      </c>
       <c r="H14" s="7"/>
-      <c r="I14" s="8"/>
+      <c r="I14" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="156.75">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+    </row>
+    <row r="16" spans="1:9" ht="99.75">
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="185.25">
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="H17" s="10"/>
+      <c r="I17" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="142.5">
+      <c r="A18" s="4">
+        <v>17</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="H18" s="10"/>
+      <c r="I18" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="85.5">
+      <c r="A19" s="4">
+        <v>18</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="H19" s="10"/>
+      <c r="I19" s="11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="128.25">
+      <c r="A20" s="4">
+        <v>19</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="I20" s="10"/>
+    </row>
+    <row r="21" spans="1:9" ht="142.5">
+      <c r="A21" s="4">
+        <v>20</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="199.5">
+      <c r="A22" s="4">
+        <v>21</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="114">
+      <c r="A23" s="4">
+        <v>22</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="H23" s="10"/>
+      <c r="I23" s="11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="4">
+        <v>23</v>
+      </c>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="4">
+        <v>24</v>
+      </c>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="4">
+        <v>25</v>
+      </c>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="4">
+        <v>26</v>
+      </c>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="4">
+        <v>27</v>
+      </c>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1"/>
     <hyperlink ref="I12" r:id="rId2"/>
     <hyperlink ref="I13" r:id="rId3"/>
+    <hyperlink ref="I14" r:id="rId4"/>
+    <hyperlink ref="I17" r:id="rId5"/>
+    <hyperlink ref="I18" r:id="rId6"/>
+    <hyperlink ref="I19" r:id="rId7"/>
+    <hyperlink ref="I21" r:id="rId8"/>
+    <hyperlink ref="I23" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>